<commit_message>
Bola Spesial bisa ke-sync
</commit_message>
<xml_diff>
--- a/BukuStuff/Diagram/Dodleh.xlsx
+++ b/BukuStuff/Diagram/Dodleh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\TAGaming\BukuStuff\Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAFDF70-E845-4986-8104-587452FB6DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2B388A-56A0-41C0-9544-49AAA2E105F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{D60A3887-9EB0-4C25-AE85-6EE7ECDD4A1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D60A3887-9EB0-4C25-AE85-6EE7ECDD4A1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Width = 2</t>
   </si>
@@ -41,12 +41,21 @@
   <si>
     <t>V</t>
   </si>
+  <si>
+    <t>Swap?</t>
+  </si>
+  <si>
+    <t>Kromosom 1</t>
+  </si>
+  <si>
+    <t>Kromosom 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,8 +63,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -71,6 +94,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,7 +396,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -392,6 +436,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -700,18 +749,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A72FE7-E1A4-43FA-9B8A-9DBF00470E21}">
-  <dimension ref="H1:BH47"/>
+  <dimension ref="H1:BW47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W36" workbookViewId="0">
-      <selection activeCell="X32" sqref="X32"/>
+    <sheetView tabSelected="1" topLeftCell="BB27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="BY50" sqref="BY50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="25" max="62" width="3.28515625" customWidth="1"/>
+    <col min="64" max="64" width="12.5703125" customWidth="1"/>
+    <col min="66" max="75" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="1" spans="8:60">
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
@@ -749,7 +800,7 @@
       <c r="BG1" s="1"/>
       <c r="BH1" s="1"/>
     </row>
-    <row r="2" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="2" spans="8:60">
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
@@ -787,7 +838,7 @@
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
     </row>
-    <row r="3" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="3" spans="8:60">
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
@@ -825,7 +876,7 @@
       <c r="BG3" s="1"/>
       <c r="BH3" s="1"/>
     </row>
-    <row r="4" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="4" spans="8:60">
       <c r="Y4" s="1"/>
       <c r="Z4" s="24">
         <v>1</v>
@@ -903,7 +954,7 @@
       <c r="BG4" s="1"/>
       <c r="BH4" s="1"/>
     </row>
-    <row r="5" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="5" spans="8:60">
       <c r="Y5" s="1"/>
       <c r="Z5" s="6">
         <v>1</v>
@@ -981,7 +1032,7 @@
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
     </row>
-    <row r="6" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="6" spans="8:60">
       <c r="Y6" s="1"/>
       <c r="Z6" s="6">
         <v>0</v>
@@ -1059,7 +1110,7 @@
       <c r="BG6" s="1"/>
       <c r="BH6" s="1"/>
     </row>
-    <row r="7" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="7" spans="8:60">
       <c r="Y7" s="1"/>
       <c r="Z7" s="6">
         <v>1</v>
@@ -1137,7 +1188,7 @@
       <c r="BG7" s="1"/>
       <c r="BH7" s="1"/>
     </row>
-    <row r="8" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="8" spans="8:60">
       <c r="Y8" s="1"/>
       <c r="Z8" s="25">
         <v>1</v>
@@ -1215,7 +1266,7 @@
       <c r="BG8" s="1"/>
       <c r="BH8" s="1"/>
     </row>
-    <row r="9" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:60">
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
@@ -1253,7 +1304,7 @@
       <c r="BG9" s="1"/>
       <c r="BH9" s="1"/>
     </row>
-    <row r="10" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:60">
       <c r="H10" s="27" t="s">
         <v>0</v>
       </c>
@@ -1299,7 +1350,7 @@
       <c r="BG10" s="1"/>
       <c r="BH10" s="1"/>
     </row>
-    <row r="11" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="11" spans="8:60">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1341,7 +1392,7 @@
       <c r="BG11" s="1"/>
       <c r="BH11" s="1"/>
     </row>
-    <row r="12" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:60">
       <c r="H12" s="1">
         <v>12</v>
       </c>
@@ -1391,7 +1442,7 @@
       <c r="BG12" s="1"/>
       <c r="BH12" s="1"/>
     </row>
-    <row r="13" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:60">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1433,7 +1484,7 @@
       <c r="BG13" s="1"/>
       <c r="BH13" s="1"/>
     </row>
-    <row r="14" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="14" spans="8:60">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1475,7 +1526,7 @@
       <c r="BG14" s="1"/>
       <c r="BH14" s="1"/>
     </row>
-    <row r="15" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="15" spans="8:60">
       <c r="H15" s="2">
         <v>12</v>
       </c>
@@ -1541,7 +1592,7 @@
       <c r="BG15" s="1"/>
       <c r="BH15" s="1"/>
     </row>
-    <row r="16" spans="8:60" x14ac:dyDescent="0.25">
+    <row r="16" spans="8:60">
       <c r="H16" s="2">
         <v>-24</v>
       </c>
@@ -1603,7 +1654,7 @@
       <c r="BG16" s="1"/>
       <c r="BH16" s="1"/>
     </row>
-    <row r="17" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:60">
       <c r="M17" s="6"/>
       <c r="N17" s="1"/>
       <c r="O17" s="10">
@@ -1655,7 +1706,7 @@
       <c r="BG17" s="1"/>
       <c r="BH17" s="1"/>
     </row>
-    <row r="18" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:60">
       <c r="M18" s="12">
         <v>0</v>
       </c>
@@ -1759,7 +1810,7 @@
       <c r="BG18" s="1"/>
       <c r="BH18" s="1"/>
     </row>
-    <row r="19" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:60">
       <c r="M19" s="14">
         <v>0</v>
       </c>
@@ -1816,13 +1867,13 @@
       <c r="AL19" s="6">
         <v>0</v>
       </c>
-      <c r="AM19" s="33">
-        <v>0</v>
-      </c>
-      <c r="AN19" s="33">
-        <v>0</v>
-      </c>
-      <c r="AO19" s="33">
+      <c r="AM19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="1">
         <v>0</v>
       </c>
       <c r="AP19" s="7">
@@ -1867,7 +1918,7 @@
       <c r="BG19" s="1"/>
       <c r="BH19" s="1"/>
     </row>
-    <row r="20" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:60">
       <c r="M20" s="12">
         <v>0</v>
       </c>
@@ -1926,13 +1977,13 @@
       <c r="AL20" s="6">
         <v>1</v>
       </c>
-      <c r="AM20" s="33">
-        <v>1</v>
-      </c>
-      <c r="AN20" s="33">
-        <v>1</v>
-      </c>
-      <c r="AO20" s="33">
+      <c r="AM20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="1">
         <v>1</v>
       </c>
       <c r="AP20" s="7">
@@ -1977,7 +2028,7 @@
       <c r="BG20" s="1"/>
       <c r="BH20" s="1"/>
     </row>
-    <row r="21" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:60">
       <c r="M21" s="12">
         <v>0</v>
       </c>
@@ -2030,13 +2081,13 @@
       <c r="AL21" s="6">
         <v>0</v>
       </c>
-      <c r="AM21" s="33">
-        <v>0</v>
-      </c>
-      <c r="AN21" s="33">
-        <v>0</v>
-      </c>
-      <c r="AO21" s="33">
+      <c r="AM21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="1">
         <v>0</v>
       </c>
       <c r="AP21" s="7">
@@ -2081,7 +2132,7 @@
       <c r="BG21" s="1"/>
       <c r="BH21" s="1"/>
     </row>
-    <row r="22" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:60">
       <c r="M22" s="12">
         <v>0</v>
       </c>
@@ -2185,7 +2236,7 @@
       <c r="BG22" s="1"/>
       <c r="BH22" s="1"/>
     </row>
-    <row r="23" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:60">
       <c r="M23" s="12">
         <v>0</v>
       </c>
@@ -2239,7 +2290,7 @@
       <c r="BG23" s="1"/>
       <c r="BH23" s="1"/>
     </row>
-    <row r="24" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:60">
       <c r="M24" s="14">
         <v>0</v>
       </c>
@@ -2337,7 +2388,7 @@
       <c r="BG24" s="1"/>
       <c r="BH24" s="1"/>
     </row>
-    <row r="25" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:60">
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
@@ -2405,7 +2456,7 @@
       <c r="BG25" s="1"/>
       <c r="BH25" s="1"/>
     </row>
-    <row r="26" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:60">
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
@@ -2473,7 +2524,7 @@
       <c r="BG26" s="1"/>
       <c r="BH26" s="1"/>
     </row>
-    <row r="27" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:60">
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
@@ -2541,7 +2592,7 @@
       <c r="BG27" s="1"/>
       <c r="BH27" s="1"/>
     </row>
-    <row r="28" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:60">
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
@@ -2609,7 +2660,7 @@
       <c r="BG28" s="1"/>
       <c r="BH28" s="1"/>
     </row>
-    <row r="29" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:60">
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
@@ -2647,7 +2698,7 @@
       <c r="BG29" s="1"/>
       <c r="BH29" s="1"/>
     </row>
-    <row r="30" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:60">
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
@@ -2685,7 +2736,7 @@
       <c r="BG30" s="1"/>
       <c r="BH30" s="1"/>
     </row>
-    <row r="31" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:60">
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
@@ -2723,7 +2774,7 @@
       <c r="BG31" s="1"/>
       <c r="BH31" s="1"/>
     </row>
-    <row r="32" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:60">
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2774,7 +2825,7 @@
       <c r="BG32" s="1"/>
       <c r="BH32" s="1"/>
     </row>
-    <row r="33" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:75">
       <c r="I33" s="1"/>
       <c r="J33" s="19">
         <v>1</v>
@@ -2840,8 +2891,41 @@
       <c r="BF33" s="1"/>
       <c r="BG33" s="1"/>
       <c r="BH33" s="1"/>
-    </row>
-    <row r="34" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BL33" t="s">
+        <v>6</v>
+      </c>
+      <c r="BN33" s="33">
+        <v>10</v>
+      </c>
+      <c r="BO33" s="34">
+        <v>7</v>
+      </c>
+      <c r="BP33" s="34">
+        <v>3</v>
+      </c>
+      <c r="BQ33" s="34">
+        <v>2</v>
+      </c>
+      <c r="BR33" s="34">
+        <v>10</v>
+      </c>
+      <c r="BS33" s="34">
+        <v>5</v>
+      </c>
+      <c r="BT33" s="34">
+        <v>2</v>
+      </c>
+      <c r="BU33" s="34">
+        <v>8</v>
+      </c>
+      <c r="BV33" s="34">
+        <v>10</v>
+      </c>
+      <c r="BW33" s="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="9:75">
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -2891,8 +2975,41 @@
       <c r="BF34" s="1"/>
       <c r="BG34" s="1"/>
       <c r="BH34" s="1"/>
-    </row>
-    <row r="35" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BL34" t="s">
+        <v>7</v>
+      </c>
+      <c r="BN34" s="34">
+        <v>7</v>
+      </c>
+      <c r="BO34" s="34">
+        <v>4</v>
+      </c>
+      <c r="BP34" s="34">
+        <v>8</v>
+      </c>
+      <c r="BQ34" s="34">
+        <v>7</v>
+      </c>
+      <c r="BR34" s="34">
+        <v>4</v>
+      </c>
+      <c r="BS34" s="34">
+        <v>3</v>
+      </c>
+      <c r="BT34" s="34">
+        <v>5</v>
+      </c>
+      <c r="BU34" s="34">
+        <v>8</v>
+      </c>
+      <c r="BV34" s="34">
+        <v>8</v>
+      </c>
+      <c r="BW34" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:75">
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2942,8 +3059,18 @@
       <c r="BF35" s="1"/>
       <c r="BG35" s="1"/>
       <c r="BH35" s="1"/>
-    </row>
-    <row r="36" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BN35" s="34"/>
+      <c r="BO35" s="34"/>
+      <c r="BP35" s="34"/>
+      <c r="BQ35" s="34"/>
+      <c r="BR35" s="34"/>
+      <c r="BS35" s="34"/>
+      <c r="BT35" s="34"/>
+      <c r="BU35" s="34"/>
+      <c r="BV35" s="34"/>
+      <c r="BW35" s="34"/>
+    </row>
+    <row r="36" spans="9:75">
       <c r="I36" s="1"/>
       <c r="J36" s="19">
         <v>1</v>
@@ -3009,8 +3136,41 @@
       <c r="BF36" s="1"/>
       <c r="BG36" s="1"/>
       <c r="BH36" s="1"/>
-    </row>
-    <row r="37" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BL36" t="s">
+        <v>5</v>
+      </c>
+      <c r="BN36" s="36">
+        <v>0</v>
+      </c>
+      <c r="BO36" s="35">
+        <v>1</v>
+      </c>
+      <c r="BP36" s="36">
+        <v>0</v>
+      </c>
+      <c r="BQ36" s="35">
+        <v>1</v>
+      </c>
+      <c r="BR36" s="35">
+        <v>1</v>
+      </c>
+      <c r="BS36" s="35">
+        <v>1</v>
+      </c>
+      <c r="BT36" s="35">
+        <v>1</v>
+      </c>
+      <c r="BU36" s="35">
+        <v>1</v>
+      </c>
+      <c r="BV36" s="36">
+        <v>0</v>
+      </c>
+      <c r="BW36" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="9:75">
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -3058,8 +3218,18 @@
       <c r="BF37" s="1"/>
       <c r="BG37" s="1"/>
       <c r="BH37" s="1"/>
-    </row>
-    <row r="38" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BN37" s="34"/>
+      <c r="BO37" s="34"/>
+      <c r="BP37" s="34"/>
+      <c r="BQ37" s="34"/>
+      <c r="BR37" s="34"/>
+      <c r="BS37" s="34"/>
+      <c r="BT37" s="34"/>
+      <c r="BU37" s="34"/>
+      <c r="BV37" s="34"/>
+      <c r="BW37" s="34"/>
+    </row>
+    <row r="38" spans="9:75">
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
@@ -3096,8 +3266,20 @@
       <c r="BF38" s="1"/>
       <c r="BG38" s="1"/>
       <c r="BH38" s="1"/>
-    </row>
-    <row r="39" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BN38" s="34"/>
+      <c r="BO38" s="34"/>
+      <c r="BP38" s="34"/>
+      <c r="BQ38" s="34"/>
+      <c r="BR38" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS38" s="34"/>
+      <c r="BT38" s="34"/>
+      <c r="BU38" s="34"/>
+      <c r="BV38" s="34"/>
+      <c r="BW38" s="34"/>
+    </row>
+    <row r="39" spans="9:75">
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
@@ -3134,8 +3316,18 @@
       <c r="BF39" s="1"/>
       <c r="BG39" s="1"/>
       <c r="BH39" s="1"/>
-    </row>
-    <row r="40" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BN39" s="34"/>
+      <c r="BO39" s="34"/>
+      <c r="BP39" s="34"/>
+      <c r="BQ39" s="34"/>
+      <c r="BR39" s="34"/>
+      <c r="BS39" s="34"/>
+      <c r="BT39" s="34"/>
+      <c r="BU39" s="34"/>
+      <c r="BV39" s="34"/>
+      <c r="BW39" s="34"/>
+    </row>
+    <row r="40" spans="9:75">
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
@@ -3172,8 +3364,41 @@
       <c r="BF40" s="1"/>
       <c r="BG40" s="1"/>
       <c r="BH40" s="1"/>
-    </row>
-    <row r="41" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BL40" t="s">
+        <v>6</v>
+      </c>
+      <c r="BN40" s="33">
+        <v>10</v>
+      </c>
+      <c r="BO40" s="34">
+        <v>4</v>
+      </c>
+      <c r="BP40" s="34">
+        <v>3</v>
+      </c>
+      <c r="BQ40" s="34">
+        <v>7</v>
+      </c>
+      <c r="BR40" s="34">
+        <v>4</v>
+      </c>
+      <c r="BS40" s="34">
+        <v>3</v>
+      </c>
+      <c r="BT40" s="34">
+        <v>5</v>
+      </c>
+      <c r="BU40" s="34">
+        <v>8</v>
+      </c>
+      <c r="BV40" s="34">
+        <v>10</v>
+      </c>
+      <c r="BW40" s="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="9:75">
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
@@ -3210,8 +3435,41 @@
       <c r="BF41" s="1"/>
       <c r="BG41" s="1"/>
       <c r="BH41" s="1"/>
-    </row>
-    <row r="42" spans="9:60" x14ac:dyDescent="0.25">
+      <c r="BL41" t="s">
+        <v>7</v>
+      </c>
+      <c r="BN41" s="34">
+        <v>7</v>
+      </c>
+      <c r="BO41" s="34">
+        <v>7</v>
+      </c>
+      <c r="BP41" s="34">
+        <v>8</v>
+      </c>
+      <c r="BQ41" s="34">
+        <v>2</v>
+      </c>
+      <c r="BR41" s="34">
+        <v>10</v>
+      </c>
+      <c r="BS41" s="34">
+        <v>5</v>
+      </c>
+      <c r="BT41" s="34">
+        <v>2</v>
+      </c>
+      <c r="BU41" s="34">
+        <v>8</v>
+      </c>
+      <c r="BV41" s="34">
+        <v>8</v>
+      </c>
+      <c r="BW41" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="9:75">
       <c r="Y42" s="1"/>
       <c r="Z42" s="24">
         <v>0</v>
@@ -3299,7 +3557,7 @@
       <c r="BG42" s="1"/>
       <c r="BH42" s="1"/>
     </row>
-    <row r="43" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:75">
       <c r="Y43" s="1"/>
       <c r="Z43" s="6">
         <v>0</v>
@@ -3387,7 +3645,7 @@
       <c r="BG43" s="1"/>
       <c r="BH43" s="1"/>
     </row>
-    <row r="44" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:75">
       <c r="Y44" s="1"/>
       <c r="Z44" s="6">
         <v>0</v>
@@ -3475,7 +3733,7 @@
       <c r="BG44" s="1"/>
       <c r="BH44" s="1"/>
     </row>
-    <row r="45" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:75">
       <c r="Y45" s="1"/>
       <c r="Z45" s="6">
         <v>0</v>
@@ -3563,7 +3821,7 @@
       <c r="BG45" s="1"/>
       <c r="BH45" s="1"/>
     </row>
-    <row r="46" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:75">
       <c r="Y46" s="1"/>
       <c r="Z46" s="25">
         <v>0</v>
@@ -3651,7 +3909,7 @@
       <c r="BG46" s="1"/>
       <c r="BH46" s="1"/>
     </row>
-    <row r="47" spans="9:60" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:75">
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>

</xml_diff>